<commit_message>
More debugging with Franco
</commit_message>
<xml_diff>
--- a/test_inputs/out3.xlsx
+++ b/test_inputs/out3.xlsx
@@ -3,7 +3,7 @@
 <s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <s:workbookPr codeName="ThisWorkbook"/>
   <s:bookViews>
-    <s:workbookView activeTab="1"/>
+    <s:workbookView activeTab="2"/>
   </s:bookViews>
   <s:sheets>
     <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,22 @@
     <t>Here's some formatting</t>
   </si>
   <si>
-    <t>A table</t>
-  </si>
-  <si>
-    <t>Column 1</t>
-  </si>
-  <si>
-    <t>Column 2</t>
-  </si>
-  <si>
-    <t>Column 3</t>
-  </si>
-  <si>
-    <t>Column 4</t>
-  </si>
-  <si>
-    <t>Column 5</t>
+    <t>a table</t>
+  </si>
+  <si>
+    <t>column 1</t>
+  </si>
+  <si>
+    <t>column 2</t>
+  </si>
+  <si>
+    <t>column 3</t>
+  </si>
+  <si>
+    <t>column 4</t>
+  </si>
+  <si>
+    <t>column 5</t>
   </si>
   <si>
     <t>AZ</t>
@@ -146,7 +146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -154,43 +154,16 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF66CCFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.5999938962981048"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -198,121 +171,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -613,145 +477,76 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="9" width="22.140625"/>
-    <col max="2" min="2" style="9"/>
-    <col max="3" min="3" style="9"/>
-    <col max="4" min="4" style="9"/>
-    <col max="5" min="5" style="9"/>
-    <col max="6" min="6" style="9"/>
-  </cols>
   <sheetData>
-    <row s="9" r="1" spans="1:6">
-      <c s="2" r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="B1" t="n"/>
-      <c s="1" r="C1" t="n"/>
-      <c s="1" r="D1" t="n"/>
-      <c s="1" r="E1" t="n"/>
-      <c s="1" r="F1" t="n"/>
-    </row>
-    <row s="9" r="2" spans="1:6">
-      <c s="3" r="A2" t="n"/>
-      <c s="3" r="B2" t="n"/>
-      <c s="3" r="C2" t="n"/>
-      <c s="3" r="D2" t="n"/>
-      <c s="3" r="E2" t="n"/>
-      <c s="3" r="F2" t="n"/>
-    </row>
-    <row s="9" r="3" spans="1:6">
-      <c s="3" r="A3" t="n"/>
-      <c s="14" r="B3" t="n">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="B3" t="n">
         <v>2</v>
       </c>
-      <c s="14" r="C3" t="n"/>
-      <c s="14" r="D3" t="n">
+      <c r="D3" t="n">
         <v>4</v>
       </c>
-      <c s="14" r="E3" t="n"/>
-      <c s="14" r="F3" t="n">
+      <c r="F3" t="n">
         <v>6</v>
       </c>
     </row>
-    <row s="9" r="4" spans="1:6">
-      <c s="3" r="A4" t="n"/>
-      <c s="14" r="B4" t="n">
+    <row r="4" spans="1:6">
+      <c r="B4" t="n">
         <v>3</v>
       </c>
-      <c s="14" r="C4" t="n"/>
-      <c s="14" r="D4" t="n">
+      <c r="D4" t="n">
         <v>6</v>
       </c>
-      <c s="14" r="E4" t="n"/>
-      <c s="14" r="F4" t="n">
+      <c r="F4" t="n">
         <v>9</v>
       </c>
     </row>
-    <row s="9" r="5" spans="1:6">
-      <c s="3" r="A5" t="n"/>
-      <c s="14" r="B5" t="n"/>
-      <c s="14" r="C5" t="n"/>
-      <c s="14" r="D5" t="n"/>
-      <c s="14" r="E5" t="n"/>
-      <c s="14" r="F5" t="n"/>
-    </row>
-    <row s="9" r="6" spans="1:6">
-      <c s="3" r="A6" t="n"/>
-      <c s="14" r="B6" t="n">
+    <row r="6" spans="1:6">
+      <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c s="14" r="C6" t="n"/>
-      <c s="14" r="D6" t="n">
+      <c r="D6" t="n">
         <v>8</v>
       </c>
-      <c s="14" r="E6" t="n"/>
-      <c s="14" r="F6" t="n">
+      <c r="F6" t="n">
         <v>12</v>
       </c>
     </row>
-    <row s="9" r="7" spans="1:6">
-      <c s="3" r="A7" t="n"/>
-      <c s="14" r="B7" t="n"/>
-      <c s="14" r="C7" t="n"/>
-      <c s="14" r="D7" t="n"/>
-      <c s="14" r="E7" t="n"/>
-      <c s="14" r="F7" t="n"/>
-    </row>
-    <row s="9" r="8" spans="1:6">
-      <c s="3" r="A8" t="n"/>
-      <c s="14" r="B8" t="n">
+    <row r="8" spans="1:6">
+      <c r="B8" t="n">
         <v>5</v>
       </c>
-      <c s="14" r="C8" t="n"/>
-      <c s="14" r="D8" t="n">
+      <c r="D8" t="n">
         <v>10</v>
       </c>
-      <c s="14" r="E8" t="n"/>
-      <c s="14" r="F8" t="n">
+      <c r="F8" t="n">
         <v>15</v>
       </c>
     </row>
-    <row s="9" r="9" spans="1:6">
-      <c s="3" r="A9" t="n"/>
-      <c s="14" r="B9" t="n"/>
-      <c s="14" r="C9" t="n"/>
-      <c s="14" r="D9" t="n"/>
-      <c s="14" r="E9" t="n"/>
-      <c s="14" r="F9" t="n"/>
-    </row>
-    <row s="9" r="10" spans="1:6">
-      <c s="3" r="A10" t="n"/>
-      <c s="14" r="B10" t="n">
+    <row r="10" spans="1:6">
+      <c r="B10" t="n">
         <v>6</v>
       </c>
-      <c s="14" r="C10" t="n"/>
-      <c s="14" r="D10" t="n">
+      <c r="D10" t="n">
         <v>12</v>
       </c>
-      <c s="14" r="E10" t="n"/>
-      <c s="14" r="F10" t="n">
+      <c r="F10" t="n">
         <v>18</v>
       </c>
-    </row>
-    <row s="9" r="11" spans="1:6">
-      <c s="3" r="A11" t="n"/>
-      <c s="14" r="B11" t="n"/>
-      <c s="14" r="C11" t="n"/>
-      <c s="14" r="D11" t="n"/>
-      <c s="14" r="E11" t="n"/>
-      <c s="14" r="F11" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -761,333 +556,295 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col customWidth="1" max="1" min="1" style="9" width="12.5703125"/>
-    <col max="2" min="2" style="9"/>
-    <col max="3" min="3" style="9"/>
-    <col max="4" min="4" style="9"/>
-    <col max="5" min="5" style="9"/>
-    <col max="6" min="6" style="9"/>
-  </cols>
   <sheetData>
-    <row s="9" r="1" spans="1:6">
-      <c s="4" r="A1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c s="4" r="B1" t="n"/>
-      <c s="4" r="C1" t="n"/>
-      <c s="4" r="D1" t="n"/>
-      <c s="4" r="E1" t="n"/>
-      <c s="4" r="F1" t="n"/>
-    </row>
-    <row s="9" r="2" spans="1:6">
-      <c s="4" r="A2" t="n"/>
-      <c s="4" r="B2" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c s="4" r="C2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c s="4" r="D2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c s="4" r="E2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c s="4" r="F2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row s="9" r="3" spans="1:6">
-      <c s="4" r="A3" t="n"/>
-      <c s="4" r="B3" t="n"/>
-      <c s="4" r="C3" t="n"/>
-      <c s="4" r="D3" t="n"/>
-      <c s="4" r="E3" t="n"/>
-      <c s="4" r="F3" t="n"/>
-    </row>
-    <row s="9" r="4" spans="1:6">
-      <c s="4" r="A4" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c s="4" r="B4" t="n">
+      <c r="B4" t="n">
         <v>2013</v>
       </c>
-      <c s="4" r="C4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D4" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c s="4" r="E4" t="n">
+      <c r="E4" t="n">
         <v>3</v>
       </c>
-      <c s="4" r="F4" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row s="9" r="5" spans="1:6">
-      <c s="4" r="A5" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c s="4" r="B5" t="n">
+      <c r="B5" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c s="4" r="D5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c s="4" r="E5" t="n">
+      <c r="E5" t="n">
         <v>4</v>
       </c>
-      <c s="4" r="F5" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row s="9" r="6" spans="1:6">
-      <c s="4" r="A6" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c s="4" r="B6" t="n">
+      <c r="B6" t="n">
         <v>2013</v>
       </c>
-      <c s="4" r="C6" t="s">
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D6" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c s="4" r="E6" t="n">
+      <c r="E6" t="n">
         <v>5</v>
       </c>
-      <c s="4" r="F6" t="s">
+      <c r="F6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row s="9" r="7" spans="1:6">
-      <c s="4" r="A7" t="s">
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c s="4" r="B7" t="n">
+      <c r="B7" t="n">
         <v>2013</v>
       </c>
-      <c s="4" r="C7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
-      <c s="4" r="D7" t="s">
+      <c r="D7" t="s">
         <v>19</v>
       </c>
-      <c s="4" r="E7" t="n">
+      <c r="E7" t="n">
         <v>6</v>
       </c>
-      <c s="4" r="F7" t="s">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row s="9" r="8" spans="1:6">
-      <c s="4" r="A8" t="s">
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c s="4" r="B8" t="n">
+      <c r="B8" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C8" t="s">
+      <c r="C8" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D8" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c s="4" r="E8" t="n">
+      <c r="E8" t="n">
         <v>7</v>
       </c>
-      <c s="4" r="F8" t="s">
+      <c r="F8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row s="9" r="9" spans="1:6">
-      <c s="4" r="A9" t="s">
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>23</v>
       </c>
-      <c s="4" r="B9" t="n">
+      <c r="B9" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C9" t="s">
+      <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c s="4" r="D9" t="s">
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c s="4" r="E9" t="n">
+      <c r="E9" t="n">
         <v>8</v>
       </c>
-      <c s="4" r="F9" t="s">
+      <c r="F9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row s="9" r="10" spans="1:6">
-      <c s="4" r="A10" t="s">
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c s="4" r="B10" t="n">
+      <c r="B10" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C10" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D10" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c s="4" r="E10" t="n">
+      <c r="E10" t="n">
         <v>9</v>
       </c>
-      <c s="4" r="F10" t="s">
+      <c r="F10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row s="9" r="11" spans="1:6">
-      <c s="4" r="A11" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c s="4" r="B11" t="n">
+      <c r="B11" t="n">
         <v>2013</v>
       </c>
-      <c s="4" r="C11" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c s="4" r="D11" t="s">
+      <c r="D11" t="s">
         <v>28</v>
       </c>
-      <c s="4" r="E11" t="n">
+      <c r="E11" t="n">
         <v>10</v>
       </c>
-      <c s="4" r="F11" t="s">
+      <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row s="9" r="12" spans="1:6">
-      <c s="4" r="A12" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
         <v>29</v>
       </c>
-      <c s="4" r="B12" t="n">
+      <c r="B12" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C12" t="s">
+      <c r="C12" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D12" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c s="4" r="E12" t="n">
+      <c r="E12" t="n">
         <v>11</v>
       </c>
-      <c s="4" r="F12" t="s">
+      <c r="F12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row s="9" r="13" spans="1:6">
-      <c s="4" r="A13" t="s">
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c s="4" r="B13" t="n">
+      <c r="B13" t="n">
         <v>2013</v>
       </c>
-      <c s="4" r="C13" t="s">
+      <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c s="4" r="D13" t="s">
+      <c r="D13" t="s">
         <v>32</v>
       </c>
-      <c s="4" r="E13" t="n">
+      <c r="E13" t="n">
         <v>12</v>
       </c>
-      <c s="4" r="F13" t="s">
+      <c r="F13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row s="9" r="14" spans="1:6">
-      <c s="4" r="A14" t="s">
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
-      <c s="4" r="B14" t="n">
+      <c r="B14" t="n">
         <v>2013</v>
       </c>
-      <c s="4" r="C14" t="s">
+      <c r="C14" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D14" t="s">
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c s="4" r="E14" t="n">
+      <c r="E14" t="n">
         <v>13</v>
       </c>
-      <c s="4" r="F14" t="s">
+      <c r="F14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row s="9" r="15" spans="1:6">
-      <c s="4" r="A15" t="s">
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
         <v>35</v>
       </c>
-      <c s="4" r="B15" t="n">
+      <c r="B15" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C15" t="s">
+      <c r="C15" t="s">
         <v>12</v>
       </c>
-      <c s="4" r="D15" t="s">
+      <c r="D15" t="s">
         <v>36</v>
       </c>
-      <c s="4" r="E15" t="n">
+      <c r="E15" t="n">
         <v>14</v>
       </c>
-      <c s="4" r="F15" t="s">
+      <c r="F15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row s="9" r="16" spans="1:6">
-      <c s="4" r="A16" t="s">
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
         <v>37</v>
       </c>
-      <c s="4" r="B16" t="n">
+      <c r="B16" t="n">
         <v>2012</v>
       </c>
-      <c s="4" r="C16" t="s">
+      <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c s="4" r="D16" t="s">
+      <c r="D16" t="s">
         <v>38</v>
       </c>
-      <c s="4" r="E16" t="n">
+      <c r="E16" t="n">
         <v>15</v>
       </c>
-      <c s="4" r="F16" t="s">
+      <c r="F16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row s="9" r="17" spans="1:6">
-      <c s="4" r="A17" t="n"/>
-      <c s="4" r="B17" t="n"/>
-      <c s="4" r="C17" t="n"/>
-      <c s="4" r="D17" t="n"/>
-      <c s="4" r="E17" t="n"/>
-      <c s="4" r="F17" t="n"/>
-    </row>
-    <row s="9" r="18" spans="1:6">
-      <c s="4" r="A18" t="n"/>
-      <c s="4" r="B18" t="n"/>
-      <c s="4" r="C18" t="n"/>
-      <c s="4" r="D18" t="n"/>
-      <c s="4" r="E18" t="n"/>
-      <c s="4" r="F18" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
@@ -1100,27 +857,15 @@
     <s:outlinePr summaryBelow="1" summaryRight="1"/>
     <s:pageSetUpPr/>
   </s:sheetPr>
-  <dimension ref="A2:L16"/>
+  <dimension ref="A2:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <cols>
-    <col max="2" min="2" style="9"/>
-    <col max="3" min="3" style="9"/>
-    <col max="4" min="4" style="9"/>
-    <col max="5" min="5" style="9"/>
-    <col max="6" min="6" style="9"/>
-    <col max="8" min="8" style="9"/>
-    <col max="9" min="9" style="9"/>
-    <col max="10" min="10" style="9"/>
-    <col max="11" min="11" style="9"/>
-    <col max="12" min="12" style="9"/>
-  </cols>
   <sheetData>
-    <row s="9" r="2" spans="1:12">
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>39</v>
       </c>
@@ -1128,34 +873,31 @@
         <v>40</v>
       </c>
     </row>
-    <row s="9" r="3" spans="1:12">
-      <c s="5" r="B3" t="n">
+    <row r="3" spans="1:10">
+      <c r="B3" t="n">
         <v>0.5</v>
       </c>
-      <c s="6" r="C3" t="n"/>
-      <c s="6" r="D3" t="n">
+      <c r="D3" t="n">
         <v>0.6</v>
       </c>
-      <c s="6" r="E3" t="n">
+      <c r="E3" t="n">
         <v>0.7</v>
       </c>
-      <c s="7" r="F3" t="n">
+      <c r="F3" t="n">
         <v>0.8</v>
       </c>
-      <c s="5" r="H3" t="n">
+      <c r="H3" t="n">
         <v>0.33</v>
       </c>
-      <c s="6" r="I3" t="n">
+      <c r="I3" t="n">
         <v>0.43</v>
       </c>
-      <c s="6" r="J3" t="n">
+      <c r="J3" t="n">
         <v>0.53</v>
       </c>
-      <c s="6" r="K3" t="n"/>
-      <c s="7" r="L3" t="n"/>
-    </row>
-    <row s="9" r="4" spans="1:12">
-      <c s="8" r="B4" t="n">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" t="n">
         <v>0.75</v>
       </c>
       <c r="D4" t="n">
@@ -1164,10 +906,10 @@
       <c r="E4" t="n">
         <v>1.05</v>
       </c>
-      <c s="10" r="F4" t="n">
+      <c r="F4" t="n">
         <v>1.2</v>
       </c>
-      <c s="8" r="H4" t="n">
+      <c r="H4" t="n">
         <v>0.34</v>
       </c>
       <c r="I4" t="n">
@@ -1176,10 +918,9 @@
       <c r="J4" t="n">
         <v>0.54</v>
       </c>
-      <c s="10" r="L4" t="n"/>
-    </row>
-    <row s="9" r="5" spans="1:12">
-      <c s="8" r="B5" t="n">
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" t="n">
         <v>1</v>
       </c>
       <c r="D5" t="n">
@@ -1188,10 +929,10 @@
       <c r="E5" t="n">
         <v>1.4</v>
       </c>
-      <c s="10" r="F5" t="n">
+      <c r="F5" t="n">
         <v>1.6</v>
       </c>
-      <c s="8" r="H5" t="n">
+      <c r="H5" t="n">
         <v>0.35</v>
       </c>
       <c r="I5" t="n">
@@ -1200,10 +941,9 @@
       <c r="J5" t="n">
         <v>0.55</v>
       </c>
-      <c s="10" r="L5" t="n"/>
-    </row>
-    <row s="9" r="6" spans="1:12">
-      <c s="8" r="B6" t="n">
+    </row>
+    <row r="6" spans="1:10">
+      <c r="B6" t="n">
         <v>1.25</v>
       </c>
       <c r="D6" t="n">
@@ -1212,10 +952,10 @@
       <c r="E6" t="n">
         <v>1.75</v>
       </c>
-      <c s="10" r="F6" t="n">
+      <c r="F6" t="n">
         <v>2</v>
       </c>
-      <c s="8" r="H6" t="n">
+      <c r="H6" t="n">
         <v>0.36</v>
       </c>
       <c r="I6" t="n">
@@ -1224,10 +964,9 @@
       <c r="J6" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c s="10" r="L6" t="n"/>
-    </row>
-    <row s="9" r="7" spans="1:12">
-      <c s="8" r="B7" t="n">
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" t="n">
         <v>1.5</v>
       </c>
       <c r="D7" t="n">
@@ -1236,10 +975,10 @@
       <c r="E7" t="n">
         <v>2.1</v>
       </c>
-      <c s="10" r="F7" t="n">
+      <c r="F7" t="n">
         <v>2.4</v>
       </c>
-      <c s="8" r="H7" t="n">
+      <c r="H7" t="n">
         <v>0.37</v>
       </c>
       <c r="I7" t="n">
@@ -1248,10 +987,9 @@
       <c r="J7" t="n">
         <v>0.57</v>
       </c>
-      <c s="10" r="L7" t="n"/>
-    </row>
-    <row s="9" r="8" spans="1:12">
-      <c s="8" r="B8" t="n">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="B8" t="n">
         <v>1.75</v>
       </c>
       <c r="D8" t="n">
@@ -1260,10 +998,10 @@
       <c r="E8" t="n">
         <v>2.45</v>
       </c>
-      <c s="10" r="F8" t="n">
+      <c r="F8" t="n">
         <v>2.8</v>
       </c>
-      <c s="8" r="H8" t="n">
+      <c r="H8" t="n">
         <v>0.38</v>
       </c>
       <c r="I8" t="n">
@@ -1272,10 +1010,9 @@
       <c r="J8" t="n">
         <v>0.58</v>
       </c>
-      <c s="10" r="L8" t="n"/>
-    </row>
-    <row s="9" r="9" spans="1:12">
-      <c s="8" r="B9" t="n">
+    </row>
+    <row r="9" spans="1:10">
+      <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="D9" t="n">
@@ -1284,10 +1021,10 @@
       <c r="E9" t="n">
         <v>2.8</v>
       </c>
-      <c s="10" r="F9" t="n">
+      <c r="F9" t="n">
         <v>3.2</v>
       </c>
-      <c s="8" r="H9" t="n">
+      <c r="H9" t="n">
         <v>0.39</v>
       </c>
       <c r="I9" t="n">
@@ -1296,10 +1033,9 @@
       <c r="J9" t="n">
         <v>0.59</v>
       </c>
-      <c s="10" r="L9" t="n"/>
-    </row>
-    <row s="9" r="10" spans="1:12">
-      <c s="8" r="B10" t="n">
+    </row>
+    <row r="10" spans="1:10">
+      <c r="B10" t="n">
         <v>2.25</v>
       </c>
       <c r="D10" t="n">
@@ -1308,10 +1044,10 @@
       <c r="E10" t="n">
         <v>3.15</v>
       </c>
-      <c s="10" r="F10" t="n">
+      <c r="F10" t="n">
         <v>3.6</v>
       </c>
-      <c s="8" r="H10" t="n">
+      <c r="H10" t="n">
         <v>0.4</v>
       </c>
       <c r="I10" t="n">
@@ -1320,10 +1056,9 @@
       <c r="J10" t="n">
         <v>0.6</v>
       </c>
-      <c s="10" r="L10" t="n"/>
-    </row>
-    <row s="9" r="11" spans="1:12">
-      <c s="8" r="B11" t="n">
+    </row>
+    <row r="11" spans="1:10">
+      <c r="B11" t="n">
         <v>2.5</v>
       </c>
       <c r="D11" t="n">
@@ -1332,10 +1067,10 @@
       <c r="E11" t="n">
         <v>3.5</v>
       </c>
-      <c s="10" r="F11" t="n">
+      <c r="F11" t="n">
         <v>4</v>
       </c>
-      <c s="8" r="H11" t="n">
+      <c r="H11" t="n">
         <v>0.41</v>
       </c>
       <c r="I11" t="n">
@@ -1344,10 +1079,9 @@
       <c r="J11" t="n">
         <v>0.61</v>
       </c>
-      <c s="10" r="L11" t="n"/>
-    </row>
-    <row s="9" r="12" spans="1:12">
-      <c s="8" r="B12" t="n">
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" t="n">
         <v>2.75</v>
       </c>
       <c r="D12" t="n">
@@ -1356,10 +1090,10 @@
       <c r="E12" t="n">
         <v>3.85</v>
       </c>
-      <c s="10" r="F12" t="n">
+      <c r="F12" t="n">
         <v>4.4</v>
       </c>
-      <c s="8" r="H12" t="n">
+      <c r="H12" t="n">
         <v>0.42</v>
       </c>
       <c r="I12" t="n">
@@ -1368,10 +1102,9 @@
       <c r="J12" t="n">
         <v>0.62</v>
       </c>
-      <c s="10" r="L12" t="n"/>
-    </row>
-    <row s="9" r="13" spans="1:12">
-      <c s="8" r="B13" t="n">
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" t="n">
         <v>3</v>
       </c>
       <c r="D13" t="n">
@@ -1380,10 +1113,10 @@
       <c r="E13" t="n">
         <v>4.2</v>
       </c>
-      <c s="10" r="F13" t="n">
+      <c r="F13" t="n">
         <v>4.8</v>
       </c>
-      <c s="8" r="H13" t="n">
+      <c r="H13" t="n">
         <v>0.43</v>
       </c>
       <c r="I13" t="n">
@@ -1392,10 +1125,9 @@
       <c r="J13" t="n">
         <v>0.63</v>
       </c>
-      <c s="10" r="L13" t="n"/>
-    </row>
-    <row s="9" r="14" spans="1:12">
-      <c s="8" r="B14" t="n">
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" t="n">
         <v>3.25</v>
       </c>
       <c r="D14" t="n">
@@ -1404,14 +1136,12 @@
       <c r="E14" t="n">
         <v>4.55</v>
       </c>
-      <c s="10" r="F14" t="n">
+      <c r="F14" t="n">
         <v>5.2</v>
       </c>
-      <c s="8" r="H14" t="n"/>
-      <c s="10" r="L14" t="n"/>
-    </row>
-    <row s="9" r="15" spans="1:12">
-      <c s="8" r="B15" t="n">
+    </row>
+    <row r="15" spans="1:10">
+      <c r="B15" t="n">
         <v>3.5</v>
       </c>
       <c r="D15" t="n">
@@ -1420,23 +1150,9 @@
       <c r="E15" t="n">
         <v>4.9</v>
       </c>
-      <c s="10" r="F15" t="n">
+      <c r="F15" t="n">
         <v>5.6</v>
       </c>
-      <c s="8" r="H15" t="n"/>
-      <c s="10" r="L15" t="n"/>
-    </row>
-    <row s="9" r="16" spans="1:12">
-      <c s="11" r="B16" t="n"/>
-      <c s="12" r="C16" t="n"/>
-      <c s="12" r="D16" t="n"/>
-      <c s="12" r="E16" t="n"/>
-      <c s="13" r="F16" t="n"/>
-      <c s="11" r="H16" t="n"/>
-      <c s="12" r="I16" t="n"/>
-      <c s="12" r="J16" t="n"/>
-      <c s="12" r="K16" t="n"/>
-      <c s="13" r="L16" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>